<commit_message>
finally got marraige stuff
</commit_message>
<xml_diff>
--- a/full_data/test_marriage_data.xlsx
+++ b/full_data/test_marriage_data.xlsx
@@ -370,7 +370,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>list(marriage_vector)</t>
+          <t>string_spouse</t>
         </is>
       </c>
     </row>
@@ -383,6 +383,11 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Catelynken Thomasdr  Raes (1591 - ca. 1645)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -393,6 +398,11 @@
       <c r="B3">
         <v>3</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>c("Marya   Boscoop (? - 1642)", "Helena   Heussen (1621 - 1680)", "Maria   Nooseman (1652 - 1729)")</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -403,6 +413,11 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>c("Geertje Gijsbertsdr, alias:  Giertje / Guertje Ghijsbers (1582 - ca. 1622)", "Aefje Willems  Saskers, alias:  Aafgie (1592 - ?)")</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -413,6 +428,11 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>c("Duifke  de Bruyn (1638 - 1668)", "Niesje   Mangeles (1647 - 1710)")</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -423,6 +443,11 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>c("Saertje Gerrits van Laar (1642 - 1683)", "Eva   Tol (1650 - 1727)")</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -433,6 +458,11 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Paschasia  van Geldre (? - ?)</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -443,6 +473,11 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Anneken Claesdr. de Moor (? - 1640)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -453,6 +488,11 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>c("Marguerite  van Bracht (? - 1600)", "Catharina  du Pire (ca. 1581 - 1654)")</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -462,6 +502,11 @@
       </c>
       <c r="B10">
         <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>c("Anneke Harmensdr.  Abeels (1590 - 1615)", "Lysbeth Reyniersdr. (1593 - 1675)")</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>